<commit_message>
changes for https://github.com/sust-cs-uob/dimpact-api/issues/4 - update bool handling of PintArray - finish calc handler - finish update table handler
</commit_message>
<xml_diff>
--- a/tests/test_v2.xlsx
+++ b/tests/test_v2.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1880" yWindow="3560" windowWidth="28560" windowHeight="17380" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="820" yWindow="1400" windowWidth="28560" windowHeight="17380" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" state="visible" r:id="rId1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -609,8 +609,10 @@
           <t>exp</t>
         </is>
       </c>
-      <c r="D2" t="n">
-        <v>10</v>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
       </c>
       <c r="F2" t="n">
         <v>0.4</v>

</xml_diff>

<commit_message>
added support for group variable table updates
</commit_message>
<xml_diff>
--- a/tests/test_v2.xlsx
+++ b/tests/test_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jedpreist/CodingStuff/DIMPACT/eam-data-tools/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE33B8FF-4EA3-F643-BEE9-69A2C461BA8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84DAED32-E2FC-FA43-A9FD-947462D75891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="820" yWindow="1400" windowWidth="28560" windowHeight="17380" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="1400" windowWidth="28560" windowHeight="17380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="58">
   <si>
     <t>version</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>choice</t>
+  </si>
+  <si>
+    <t>group</t>
   </si>
 </sst>
 </file>
@@ -667,21 +670,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:T18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="9" max="9" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -689,372 +692,396 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="7" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="9" t="s">
+      <c r="T1" s="9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.4</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="4">
         <v>-0.2</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="4">
         <v>0.1</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>39814</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>24</v>
       </c>
-      <c r="S2">
+      <c r="T2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.4</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="4">
         <v>-0.2</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="4">
         <v>0.1</v>
       </c>
-      <c r="J3" s="3">
+      <c r="K3" s="3">
         <v>39814</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>24</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1">
+      <c r="F4" s="1"/>
+      <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="3">
+        <v>39814</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S4">
+      <c r="T4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1"/>
+      <c r="G5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="3">
+        <v>39814</v>
+      </c>
+      <c r="L5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6">
+      <c r="F6" s="1"/>
+      <c r="G6">
         <v>1</v>
       </c>
-      <c r="S6">
+      <c r="K6" s="3">
+        <v>39814</v>
+      </c>
+      <c r="T6">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
       <c r="B7" t="s">
         <v>35</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="K7" t="s">
+      <c r="H7" s="1"/>
+      <c r="K7" s="3">
+        <v>39814</v>
+      </c>
+      <c r="L7" t="s">
         <v>24</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>36</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" t="s">
+      <c r="K8" s="3">
+        <v>39814</v>
+      </c>
+      <c r="L8" t="s">
         <v>24</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9">
+      <c r="F9" s="1"/>
+      <c r="G9">
         <v>0</v>
       </c>
-      <c r="S9">
+      <c r="K9" s="3">
+        <v>39814</v>
+      </c>
+      <c r="T9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="5">
+      <c r="G10" s="5">
         <v>123</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>40</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>0.5</v>
       </c>
-      <c r="J10" s="3">
+      <c r="K10" s="3">
         <v>42005</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="4">
         <v>0.1</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="3">
+      <c r="J11" s="4"/>
+      <c r="K11" s="3">
         <v>39448</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>24</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="4">
         <v>0.1</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="3">
+      <c r="J12" s="4"/>
+      <c r="K12" s="3">
         <v>39448</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>24</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1">
         <v>2</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="3">
+        <v>39814</v>
+      </c>
+      <c r="L13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="H14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="4">
         <v>0.1</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="J14" s="3">
+      <c r="J14" s="4"/>
+      <c r="K14" s="3">
         <v>39814</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>24</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="S15">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="T15">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="8"/>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
-      <c r="P17" s="8"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="8"/>
-      <c r="S17" s="9"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="L18" s="1"/>
-      <c r="N18" s="1"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="8"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="8"/>
+      <c r="T17" s="9"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M18" s="1"/>
       <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1064,10 +1091,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1075,7 +1102,7 @@
     <col min="1" max="1" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1083,83 +1110,86 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
         <v>46</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>48</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>55</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>56</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>39814</v>
       </c>
-      <c r="J2" s="3">
+      <c r="K2" s="3">
         <v>39904</v>
       </c>
-      <c r="K2" s="4">
+      <c r="L2" s="4">
         <v>0.1</v>
       </c>
-      <c r="L2" s="3">
+      <c r="M2" s="3">
         <v>39814</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="P2">
+      <c r="Q2">
         <v>15</v>
       </c>
     </row>

</xml_diff>